<commit_message>
Fix: Waybills page now fetches total debt directly from payments page
Instead of recalculating, waybills page now:
1. Payments page stores totalOutstanding in query cache
2. Waybills page reads it directly from cache

This ensures both pages show EXACTLY the same total debt.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boris\Dell\Projects\APPS\ERP\Tasty_erp_new\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469BABEE-E136-49EC-9C74-CB79F0FED8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385A84F9-347E-4EC5-9C36-3526AF15851F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -559,7 +570,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,14 +606,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -874,12 +898,13 @@
   <dimension ref="A1:W246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:W246"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1038,7 +1063,7 @@
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>1150</v>
       </c>
       <c r="F3">
@@ -1097,7 +1122,7 @@
       <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1035</v>
       </c>
       <c r="F4">
@@ -1156,7 +1181,7 @@
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>1150</v>
       </c>
       <c r="F5">
@@ -1218,7 +1243,7 @@
       <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1840</v>
       </c>
       <c r="F6">
@@ -1277,7 +1302,7 @@
       <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1610</v>
       </c>
       <c r="F7">
@@ -1339,7 +1364,7 @@
       <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>1955</v>
       </c>
       <c r="F8">
@@ -1401,7 +1426,7 @@
       <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>1410</v>
       </c>
       <c r="F9">
@@ -1463,7 +1488,7 @@
       <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1410</v>
       </c>
       <c r="F10">
@@ -1522,7 +1547,7 @@
       <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1410</v>
       </c>
       <c r="F11">
@@ -1581,7 +1606,7 @@
       <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>1645</v>
       </c>
       <c r="F12">
@@ -1640,7 +1665,7 @@
       <c r="D13" t="s">
         <v>46</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1175</v>
       </c>
       <c r="F13">
@@ -1699,7 +1724,7 @@
       <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>1410</v>
       </c>
       <c r="F14">
@@ -1761,7 +1786,7 @@
       <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>1410</v>
       </c>
       <c r="F15">
@@ -1823,7 +1848,7 @@
       <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>1645</v>
       </c>
       <c r="F16">
@@ -1885,7 +1910,7 @@
       <c r="D17" t="s">
         <v>46</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>1762.5</v>
       </c>
       <c r="F17">
@@ -1944,7 +1969,7 @@
       <c r="D18" t="s">
         <v>46</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>587.5</v>
       </c>
       <c r="F18">
@@ -2003,7 +2028,7 @@
       <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>940</v>
       </c>
       <c r="F19">
@@ -2065,7 +2090,7 @@
       <c r="D20" t="s">
         <v>46</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>1762.5</v>
       </c>
       <c r="F20">
@@ -2124,7 +2149,7 @@
       <c r="D21" t="s">
         <v>46</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>1292.5</v>
       </c>
       <c r="F21">
@@ -2183,7 +2208,7 @@
       <c r="D22" t="s">
         <v>46</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>2115</v>
       </c>
       <c r="F22">
@@ -2245,7 +2270,7 @@
       <c r="D23" t="s">
         <v>46</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>822.5</v>
       </c>
       <c r="F23">
@@ -2307,7 +2332,7 @@
       <c r="D24" t="s">
         <v>46</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>1175</v>
       </c>
       <c r="F24">
@@ -2366,7 +2391,7 @@
       <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>1645</v>
       </c>
       <c r="F25">
@@ -2425,7 +2450,7 @@
       <c r="D26" t="s">
         <v>46</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>1645</v>
       </c>
       <c r="F26">
@@ -2487,7 +2512,7 @@
       <c r="D27" t="s">
         <v>46</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>1175</v>
       </c>
       <c r="F27">
@@ -2546,7 +2571,7 @@
       <c r="D28" t="s">
         <v>46</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>1410</v>
       </c>
       <c r="F28">
@@ -2608,7 +2633,7 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>1762.5</v>
       </c>
       <c r="F29">
@@ -2670,7 +2695,7 @@
       <c r="D30" t="s">
         <v>46</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>2115</v>
       </c>
       <c r="F30">
@@ -2732,7 +2757,7 @@
       <c r="D31" t="s">
         <v>46</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>1645</v>
       </c>
       <c r="F31">
@@ -2794,7 +2819,7 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>1645</v>
       </c>
       <c r="F32">
@@ -2853,7 +2878,7 @@
       <c r="D33" t="s">
         <v>46</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>1175</v>
       </c>
       <c r="F33">
@@ -2915,7 +2940,7 @@
       <c r="D34" t="s">
         <v>46</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>2115</v>
       </c>
       <c r="F34">
@@ -2974,7 +2999,7 @@
       <c r="D35" t="s">
         <v>46</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>1150</v>
       </c>
       <c r="F35">
@@ -3033,7 +3058,7 @@
       <c r="D36" t="s">
         <v>46</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>1645</v>
       </c>
       <c r="F36">
@@ -3095,7 +3120,7 @@
       <c r="D37" t="s">
         <v>46</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>1610</v>
       </c>
       <c r="F37">
@@ -3154,7 +3179,7 @@
       <c r="D38" t="s">
         <v>46</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1000</v>
       </c>
       <c r="F38">
@@ -3213,7 +3238,7 @@
       <c r="D39" t="s">
         <v>46</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>1480</v>
       </c>
       <c r="F39">
@@ -3275,7 +3300,7 @@
       <c r="D40" t="s">
         <v>46</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>1840</v>
       </c>
       <c r="F40">
@@ -3334,7 +3359,7 @@
       <c r="D41" t="s">
         <v>46</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>1150</v>
       </c>
       <c r="F41">
@@ -3396,7 +3421,7 @@
       <c r="D42" t="s">
         <v>46</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>920</v>
       </c>
       <c r="F42">
@@ -3458,7 +3483,7 @@
       <c r="D43" t="s">
         <v>46</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>2760</v>
       </c>
       <c r="F43">
@@ -3517,7 +3542,7 @@
       <c r="D44" t="s">
         <v>46</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>1380</v>
       </c>
       <c r="F44">
@@ -3579,7 +3604,7 @@
       <c r="D45" t="s">
         <v>46</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>1725</v>
       </c>
       <c r="F45">
@@ -3641,7 +3666,7 @@
       <c r="D46" t="s">
         <v>46</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>1495</v>
       </c>
       <c r="F46">
@@ -3703,7 +3728,7 @@
       <c r="D47" t="s">
         <v>46</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>1495</v>
       </c>
       <c r="F47">
@@ -3762,7 +3787,7 @@
       <c r="D48" t="s">
         <v>46</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>1610</v>
       </c>
       <c r="F48">
@@ -3821,7 +3846,7 @@
       <c r="D49" t="s">
         <v>46</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>1150</v>
       </c>
       <c r="F49">
@@ -3880,7 +3905,7 @@
       <c r="D50" t="s">
         <v>46</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>920</v>
       </c>
       <c r="F50">
@@ -3942,7 +3967,7 @@
       <c r="D51" t="s">
         <v>46</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>1150</v>
       </c>
       <c r="F51">
@@ -4004,7 +4029,7 @@
       <c r="D52" t="s">
         <v>46</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>1725</v>
       </c>
       <c r="F52">
@@ -4063,7 +4088,7 @@
       <c r="D53" t="s">
         <v>46</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <v>1495</v>
       </c>
       <c r="F53">
@@ -4122,7 +4147,7 @@
       <c r="D54" t="s">
         <v>46</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>1380</v>
       </c>
       <c r="F54">
@@ -4184,7 +4209,7 @@
       <c r="D55" t="s">
         <v>46</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>1495</v>
       </c>
       <c r="F55">
@@ -4243,7 +4268,7 @@
       <c r="D56" t="s">
         <v>46</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <v>1380</v>
       </c>
       <c r="F56">
@@ -4305,7 +4330,7 @@
       <c r="D57" t="s">
         <v>46</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>1380</v>
       </c>
       <c r="F57">
@@ -4367,7 +4392,7 @@
       <c r="D58" t="s">
         <v>46</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <v>1265</v>
       </c>
       <c r="F58">
@@ -4426,7 +4451,7 @@
       <c r="D59" t="s">
         <v>46</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="2">
         <v>1495</v>
       </c>
       <c r="F59">
@@ -4488,7 +4513,7 @@
       <c r="D60" t="s">
         <v>46</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="2">
         <v>1610</v>
       </c>
       <c r="F60">
@@ -4547,7 +4572,7 @@
       <c r="D61" t="s">
         <v>46</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="2">
         <v>1035</v>
       </c>
       <c r="F61">
@@ -4606,7 +4631,7 @@
       <c r="D62" t="s">
         <v>46</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="2">
         <v>1380</v>
       </c>
       <c r="F62">
@@ -4665,7 +4690,7 @@
       <c r="D63" t="s">
         <v>46</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="2">
         <v>805</v>
       </c>
       <c r="F63">
@@ -4724,7 +4749,7 @@
       <c r="D64" t="s">
         <v>46</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="2">
         <v>1380</v>
       </c>
       <c r="F64">
@@ -4783,7 +4808,7 @@
       <c r="D65" t="s">
         <v>46</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="2">
         <v>1150</v>
       </c>
       <c r="F65">
@@ -4845,7 +4870,7 @@
       <c r="D66" t="s">
         <v>46</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="2">
         <v>1150</v>
       </c>
       <c r="F66">
@@ -4904,7 +4929,7 @@
       <c r="D67" t="s">
         <v>46</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="2">
         <v>1380</v>
       </c>
       <c r="F67">
@@ -4963,7 +4988,7 @@
       <c r="D68" t="s">
         <v>46</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="2">
         <v>1380</v>
       </c>
       <c r="F68">
@@ -5022,7 +5047,7 @@
       <c r="D69" t="s">
         <v>46</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="2">
         <v>1900</v>
       </c>
       <c r="F69">
@@ -5081,7 +5106,7 @@
       <c r="D70" t="s">
         <v>46</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="2">
         <v>1380</v>
       </c>
       <c r="F70">
@@ -5140,7 +5165,7 @@
       <c r="D71" t="s">
         <v>46</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="2">
         <v>1495</v>
       </c>
       <c r="F71">
@@ -5202,7 +5227,7 @@
       <c r="D72" t="s">
         <v>46</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="2">
         <v>1380</v>
       </c>
       <c r="F72">
@@ -5261,7 +5286,7 @@
       <c r="D73" t="s">
         <v>46</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="2">
         <v>320</v>
       </c>
       <c r="F73">
@@ -5320,7 +5345,7 @@
       <c r="D74" t="s">
         <v>46</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="2">
         <v>1220</v>
       </c>
       <c r="F74">
@@ -5382,7 +5407,7 @@
       <c r="D75" t="s">
         <v>46</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="2">
         <v>1610</v>
       </c>
       <c r="F75">
@@ -5441,7 +5466,7 @@
       <c r="D76" t="s">
         <v>46</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="2">
         <v>1500</v>
       </c>
       <c r="F76">
@@ -5500,7 +5525,7 @@
       <c r="D77" t="s">
         <v>46</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="2">
         <v>1150</v>
       </c>
       <c r="F77">
@@ -5559,7 +5584,7 @@
       <c r="D78" t="s">
         <v>46</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="2">
         <v>1380</v>
       </c>
       <c r="F78">
@@ -5618,7 +5643,7 @@
       <c r="D79" t="s">
         <v>46</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="2">
         <v>1380</v>
       </c>
       <c r="F79">
@@ -5680,7 +5705,7 @@
       <c r="D80" t="s">
         <v>46</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="2">
         <v>1150</v>
       </c>
       <c r="F80">
@@ -5742,7 +5767,7 @@
       <c r="D81" t="s">
         <v>46</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="2">
         <v>1150</v>
       </c>
       <c r="F81">
@@ -5801,7 +5826,7 @@
       <c r="D82" t="s">
         <v>46</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="2">
         <v>1380</v>
       </c>
       <c r="F82">
@@ -5860,7 +5885,7 @@
       <c r="D83" t="s">
         <v>46</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="2">
         <v>1380</v>
       </c>
       <c r="F83">
@@ -5922,7 +5947,7 @@
       <c r="D84" t="s">
         <v>46</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="2">
         <v>1265</v>
       </c>
       <c r="F84">
@@ -5981,7 +6006,7 @@
       <c r="D85" t="s">
         <v>46</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="2">
         <v>2070</v>
       </c>
       <c r="F85">
@@ -6040,7 +6065,7 @@
       <c r="D86" t="s">
         <v>46</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="2">
         <v>851</v>
       </c>
       <c r="F86">
@@ -6102,7 +6127,7 @@
       <c r="D87" t="s">
         <v>46</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="2">
         <v>1748</v>
       </c>
       <c r="F87">
@@ -6164,7 +6189,7 @@
       <c r="D88" t="s">
         <v>46</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="2">
         <v>1380</v>
       </c>
       <c r="F88">
@@ -6226,7 +6251,7 @@
       <c r="D89" t="s">
         <v>46</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="2">
         <v>920</v>
       </c>
       <c r="F89">
@@ -6285,7 +6310,7 @@
       <c r="D90" t="s">
         <v>46</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="2">
         <v>1150</v>
       </c>
       <c r="F90">
@@ -6344,7 +6369,7 @@
       <c r="D91" t="s">
         <v>46</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="2">
         <v>1380</v>
       </c>
       <c r="F91">
@@ -6406,7 +6431,7 @@
       <c r="D92" t="s">
         <v>46</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="2">
         <v>920</v>
       </c>
       <c r="F92">
@@ -6468,7 +6493,7 @@
       <c r="D93" t="s">
         <v>46</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="2">
         <v>690</v>
       </c>
       <c r="F93">
@@ -6527,7 +6552,7 @@
       <c r="D94" t="s">
         <v>46</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="2">
         <v>1610</v>
       </c>
       <c r="F94">
@@ -6586,7 +6611,7 @@
       <c r="D95" t="s">
         <v>46</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="2">
         <v>1702</v>
       </c>
       <c r="F95">
@@ -6648,7 +6673,7 @@
       <c r="D96" t="s">
         <v>46</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="2">
         <v>1725</v>
       </c>
       <c r="F96">
@@ -6707,7 +6732,7 @@
       <c r="D97" t="s">
         <v>46</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="2">
         <v>1449</v>
       </c>
       <c r="F97">
@@ -6766,7 +6791,7 @@
       <c r="D98" t="s">
         <v>46</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="2">
         <v>1610</v>
       </c>
       <c r="F98">
@@ -6828,7 +6853,7 @@
       <c r="D99" t="s">
         <v>46</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="2">
         <v>1518</v>
       </c>
       <c r="F99">
@@ -6887,7 +6912,7 @@
       <c r="D100" t="s">
         <v>46</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="2">
         <v>1150</v>
       </c>
       <c r="F100">
@@ -6949,7 +6974,7 @@
       <c r="D101" t="s">
         <v>46</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="2">
         <v>1265</v>
       </c>
       <c r="F101">
@@ -7008,7 +7033,7 @@
       <c r="D102" t="s">
         <v>46</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="2">
         <v>1150</v>
       </c>
       <c r="F102">
@@ -7067,7 +7092,7 @@
       <c r="D103" t="s">
         <v>46</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="2">
         <v>1380</v>
       </c>
       <c r="F103">
@@ -7129,7 +7154,7 @@
       <c r="D104" t="s">
         <v>46</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="2">
         <v>1150</v>
       </c>
       <c r="F104">
@@ -7191,7 +7216,7 @@
       <c r="D105" t="s">
         <v>46</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="2">
         <v>1265</v>
       </c>
       <c r="F105">
@@ -7250,7 +7275,7 @@
       <c r="D106" t="s">
         <v>46</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="2">
         <v>1265</v>
       </c>
       <c r="F106">
@@ -7309,7 +7334,7 @@
       <c r="D107" t="s">
         <v>46</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="2">
         <v>920</v>
       </c>
       <c r="F107">
@@ -7368,7 +7393,7 @@
       <c r="D108" t="s">
         <v>46</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="2">
         <v>920</v>
       </c>
       <c r="F108">
@@ -7427,7 +7452,7 @@
       <c r="D109" t="s">
         <v>46</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="2">
         <v>920</v>
       </c>
       <c r="F109">
@@ -7486,7 +7511,7 @@
       <c r="D110" t="s">
         <v>46</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="2">
         <v>1380</v>
       </c>
       <c r="F110">
@@ -7548,7 +7573,7 @@
       <c r="D111" t="s">
         <v>46</v>
       </c>
-      <c r="E111">
+      <c r="E111" s="2">
         <v>1150</v>
       </c>
       <c r="F111">
@@ -7607,7 +7632,7 @@
       <c r="D112" t="s">
         <v>46</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="2">
         <v>1150</v>
       </c>
       <c r="F112">
@@ -7666,7 +7691,7 @@
       <c r="D113" t="s">
         <v>46</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="2">
         <v>690</v>
       </c>
       <c r="F113">
@@ -7725,7 +7750,7 @@
       <c r="D114" t="s">
         <v>46</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="2">
         <v>920</v>
       </c>
       <c r="F114">
@@ -7784,7 +7809,7 @@
       <c r="D115" t="s">
         <v>46</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="2">
         <v>1150</v>
       </c>
       <c r="F115">
@@ -7846,7 +7871,7 @@
       <c r="D116" t="s">
         <v>46</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="2">
         <v>1380</v>
       </c>
       <c r="F116">
@@ -7905,7 +7930,7 @@
       <c r="D117" t="s">
         <v>46</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="2">
         <v>1150</v>
       </c>
       <c r="F117">
@@ -7964,7 +7989,7 @@
       <c r="D118" t="s">
         <v>46</v>
       </c>
-      <c r="E118">
+      <c r="E118" s="2">
         <v>1150</v>
       </c>
       <c r="F118">
@@ -8026,7 +8051,7 @@
       <c r="D119" t="s">
         <v>46</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="2">
         <v>1150</v>
       </c>
       <c r="F119">
@@ -8085,7 +8110,7 @@
       <c r="D120" t="s">
         <v>46</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="2">
         <v>1541</v>
       </c>
       <c r="F120">
@@ -8144,7 +8169,7 @@
       <c r="D121" t="s">
         <v>46</v>
       </c>
-      <c r="E121">
+      <c r="E121" s="2">
         <v>1127</v>
       </c>
       <c r="F121">
@@ -8203,7 +8228,7 @@
       <c r="D122" t="s">
         <v>46</v>
       </c>
-      <c r="E122">
+      <c r="E122" s="2">
         <v>1610</v>
       </c>
       <c r="F122">
@@ -8265,7 +8290,7 @@
       <c r="D123" t="s">
         <v>46</v>
       </c>
-      <c r="E123">
+      <c r="E123" s="2">
         <v>1610</v>
       </c>
       <c r="F123">
@@ -8324,7 +8349,7 @@
       <c r="D124" t="s">
         <v>46</v>
       </c>
-      <c r="E124">
+      <c r="E124" s="2">
         <v>920</v>
       </c>
       <c r="F124">
@@ -8386,7 +8411,7 @@
       <c r="D125" t="s">
         <v>46</v>
       </c>
-      <c r="E125">
+      <c r="E125" s="2">
         <v>1739</v>
       </c>
       <c r="F125">
@@ -8445,7 +8470,7 @@
       <c r="D126" t="s">
         <v>46</v>
       </c>
-      <c r="E126">
+      <c r="E126" s="2">
         <v>1245.5</v>
       </c>
       <c r="F126">
@@ -8504,7 +8529,7 @@
       <c r="D127" t="s">
         <v>46</v>
       </c>
-      <c r="E127">
+      <c r="E127" s="2">
         <v>1292.5</v>
       </c>
       <c r="F127">
@@ -8563,7 +8588,7 @@
       <c r="D128" t="s">
         <v>46</v>
       </c>
-      <c r="E128">
+      <c r="E128" s="2">
         <v>1715.5</v>
       </c>
       <c r="F128">
@@ -8622,7 +8647,7 @@
       <c r="D129" t="s">
         <v>46</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="2">
         <v>1903.5</v>
       </c>
       <c r="F129">
@@ -8681,7 +8706,7 @@
       <c r="D130" t="s">
         <v>46</v>
       </c>
-      <c r="E130">
+      <c r="E130" s="2">
         <v>1175</v>
       </c>
       <c r="F130">
@@ -8740,7 +8765,7 @@
       <c r="D131" t="s">
         <v>46</v>
       </c>
-      <c r="E131">
+      <c r="E131" s="2">
         <v>1410</v>
       </c>
       <c r="F131">
@@ -8802,7 +8827,7 @@
       <c r="D132" t="s">
         <v>46</v>
       </c>
-      <c r="E132">
+      <c r="E132" s="2">
         <v>1410</v>
       </c>
       <c r="F132">
@@ -8861,7 +8886,7 @@
       <c r="D133" t="s">
         <v>46</v>
       </c>
-      <c r="E133">
+      <c r="E133" s="2">
         <v>1339.5</v>
       </c>
       <c r="F133">
@@ -8923,7 +8948,7 @@
       <c r="D134" t="s">
         <v>46</v>
       </c>
-      <c r="E134">
+      <c r="E134" s="2">
         <v>1527.5</v>
       </c>
       <c r="F134">
@@ -8982,7 +9007,7 @@
       <c r="D135" t="s">
         <v>46</v>
       </c>
-      <c r="E135">
+      <c r="E135" s="2">
         <v>1433.5</v>
       </c>
       <c r="F135">
@@ -9041,7 +9066,7 @@
       <c r="D136" t="s">
         <v>46</v>
       </c>
-      <c r="E136">
+      <c r="E136" s="2">
         <v>940</v>
       </c>
       <c r="F136">
@@ -9100,7 +9125,7 @@
       <c r="D137" t="s">
         <v>46</v>
       </c>
-      <c r="E137">
+      <c r="E137" s="2">
         <v>1692</v>
       </c>
       <c r="F137">
@@ -9162,7 +9187,7 @@
       <c r="D138" t="s">
         <v>46</v>
       </c>
-      <c r="E138">
+      <c r="E138" s="2">
         <v>1175</v>
       </c>
       <c r="F138">
@@ -9224,7 +9249,7 @@
       <c r="D139" t="s">
         <v>46</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="2">
         <v>1645</v>
       </c>
       <c r="F139">
@@ -9286,7 +9311,7 @@
       <c r="D140" t="s">
         <v>46</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="2">
         <v>1880</v>
       </c>
       <c r="F140">
@@ -9345,7 +9370,7 @@
       <c r="D141" t="s">
         <v>46</v>
       </c>
-      <c r="E141">
+      <c r="E141" s="2">
         <v>1175</v>
       </c>
       <c r="F141">
@@ -9407,7 +9432,7 @@
       <c r="D142" t="s">
         <v>46</v>
       </c>
-      <c r="E142">
+      <c r="E142" s="2">
         <v>1645</v>
       </c>
       <c r="F142">
@@ -9469,7 +9494,7 @@
       <c r="D143" t="s">
         <v>46</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="2">
         <v>705</v>
       </c>
       <c r="F143">
@@ -9528,7 +9553,7 @@
       <c r="D144" t="s">
         <v>46</v>
       </c>
-      <c r="E144">
+      <c r="E144" s="2">
         <v>1175</v>
       </c>
       <c r="F144">
@@ -9587,7 +9612,7 @@
       <c r="D145" t="s">
         <v>46</v>
       </c>
-      <c r="E145">
+      <c r="E145" s="2">
         <v>1175</v>
       </c>
       <c r="F145">
@@ -9649,7 +9674,7 @@
       <c r="D146" t="s">
         <v>46</v>
       </c>
-      <c r="E146">
+      <c r="E146" s="2">
         <v>1880</v>
       </c>
       <c r="F146">
@@ -9711,7 +9736,7 @@
       <c r="D147" t="s">
         <v>46</v>
       </c>
-      <c r="E147">
+      <c r="E147" s="2">
         <v>1527.5</v>
       </c>
       <c r="F147">
@@ -9770,7 +9795,7 @@
       <c r="D148" t="s">
         <v>46</v>
       </c>
-      <c r="E148">
+      <c r="E148" s="2">
         <v>1833</v>
       </c>
       <c r="F148">
@@ -9832,7 +9857,7 @@
       <c r="D149" t="s">
         <v>46</v>
       </c>
-      <c r="E149">
+      <c r="E149" s="2">
         <v>1410</v>
       </c>
       <c r="F149">
@@ -9894,7 +9919,7 @@
       <c r="D150" t="s">
         <v>46</v>
       </c>
-      <c r="E150">
+      <c r="E150" s="2">
         <v>1645</v>
       </c>
       <c r="F150">
@@ -9953,7 +9978,7 @@
       <c r="D151" t="s">
         <v>46</v>
       </c>
-      <c r="E151">
+      <c r="E151" s="2">
         <v>1527.5</v>
       </c>
       <c r="F151">
@@ -10015,7 +10040,7 @@
       <c r="D152" t="s">
         <v>46</v>
       </c>
-      <c r="E152">
+      <c r="E152" s="2">
         <v>1410</v>
       </c>
       <c r="F152">
@@ -10077,7 +10102,7 @@
       <c r="D153" t="s">
         <v>46</v>
       </c>
-      <c r="E153">
+      <c r="E153" s="2">
         <v>1410</v>
       </c>
       <c r="F153">
@@ -10139,7 +10164,7 @@
       <c r="D154" t="s">
         <v>46</v>
       </c>
-      <c r="E154">
+      <c r="E154" s="2">
         <v>1175</v>
       </c>
       <c r="F154">
@@ -10201,7 +10226,7 @@
       <c r="D155" t="s">
         <v>46</v>
       </c>
-      <c r="E155">
+      <c r="E155" s="2">
         <v>1410</v>
       </c>
       <c r="F155">
@@ -10263,7 +10288,7 @@
       <c r="D156" t="s">
         <v>46</v>
       </c>
-      <c r="E156">
+      <c r="E156" s="2">
         <v>1410</v>
       </c>
       <c r="F156">
@@ -10322,7 +10347,7 @@
       <c r="D157" t="s">
         <v>46</v>
       </c>
-      <c r="E157">
+      <c r="E157" s="2">
         <v>822.5</v>
       </c>
       <c r="F157">
@@ -10384,7 +10409,7 @@
       <c r="D158" t="s">
         <v>46</v>
       </c>
-      <c r="E158">
+      <c r="E158" s="2">
         <v>2000</v>
       </c>
       <c r="F158">
@@ -10446,7 +10471,7 @@
       <c r="D159" t="s">
         <v>46</v>
       </c>
-      <c r="E159">
+      <c r="E159" s="2">
         <v>1410</v>
       </c>
       <c r="F159">
@@ -10505,7 +10530,7 @@
       <c r="D160" t="s">
         <v>46</v>
       </c>
-      <c r="E160">
+      <c r="E160" s="2">
         <v>1410</v>
       </c>
       <c r="F160">
@@ -10567,7 +10592,7 @@
       <c r="D161" t="s">
         <v>46</v>
       </c>
-      <c r="E161">
+      <c r="E161" s="2">
         <v>1410</v>
       </c>
       <c r="F161">
@@ -10629,7 +10654,7 @@
       <c r="D162" t="s">
         <v>46</v>
       </c>
-      <c r="E162">
+      <c r="E162" s="2">
         <v>1175</v>
       </c>
       <c r="F162">
@@ -10688,7 +10713,7 @@
       <c r="D163" t="s">
         <v>46</v>
       </c>
-      <c r="E163">
+      <c r="E163" s="2">
         <v>1175</v>
       </c>
       <c r="F163">
@@ -10750,7 +10775,7 @@
       <c r="D164" t="s">
         <v>46</v>
       </c>
-      <c r="E164">
+      <c r="E164" s="2">
         <v>1527.5</v>
       </c>
       <c r="F164">
@@ -10812,7 +10837,7 @@
       <c r="D165" t="s">
         <v>46</v>
       </c>
-      <c r="E165">
+      <c r="E165" s="2">
         <v>1410</v>
       </c>
       <c r="F165">
@@ -10874,7 +10899,7 @@
       <c r="D166" t="s">
         <v>46</v>
       </c>
-      <c r="E166">
+      <c r="E166" s="2">
         <v>1292.5</v>
       </c>
       <c r="F166">
@@ -10933,7 +10958,7 @@
       <c r="D167" t="s">
         <v>46</v>
       </c>
-      <c r="E167">
+      <c r="E167" s="2">
         <v>1880</v>
       </c>
       <c r="F167">
@@ -10995,7 +11020,7 @@
       <c r="D168" t="s">
         <v>46</v>
       </c>
-      <c r="E168">
+      <c r="E168" s="2">
         <v>1551</v>
       </c>
       <c r="F168">
@@ -11057,7 +11082,7 @@
       <c r="D169" t="s">
         <v>46</v>
       </c>
-      <c r="E169">
+      <c r="E169" s="2">
         <v>1175</v>
       </c>
       <c r="F169">
@@ -11116,7 +11141,7 @@
       <c r="D170" t="s">
         <v>46</v>
       </c>
-      <c r="E170">
+      <c r="E170" s="2">
         <v>1175</v>
       </c>
       <c r="F170">
@@ -11175,7 +11200,7 @@
       <c r="D171" t="s">
         <v>46</v>
       </c>
-      <c r="E171">
+      <c r="E171" s="2">
         <v>1175</v>
       </c>
       <c r="F171">
@@ -11237,7 +11262,7 @@
       <c r="D172" t="s">
         <v>46</v>
       </c>
-      <c r="E172">
+      <c r="E172" s="2">
         <v>1527.5</v>
       </c>
       <c r="F172">
@@ -11296,7 +11321,7 @@
       <c r="D173" t="s">
         <v>46</v>
       </c>
-      <c r="E173">
+      <c r="E173" s="2">
         <v>3000</v>
       </c>
       <c r="F173">
@@ -11358,7 +11383,7 @@
       <c r="D174" t="s">
         <v>46</v>
       </c>
-      <c r="E174">
+      <c r="E174" s="2">
         <v>1762.5</v>
       </c>
       <c r="F174">
@@ -11417,7 +11442,7 @@
       <c r="D175" t="s">
         <v>46</v>
       </c>
-      <c r="E175">
+      <c r="E175" s="2">
         <v>1645</v>
       </c>
       <c r="F175">
@@ -11476,7 +11501,7 @@
       <c r="D176" t="s">
         <v>46</v>
       </c>
-      <c r="E176">
+      <c r="E176" s="2">
         <v>1528</v>
       </c>
       <c r="F176">
@@ -11535,7 +11560,7 @@
       <c r="D177" t="s">
         <v>46</v>
       </c>
-      <c r="E177">
+      <c r="E177" s="2">
         <v>1410</v>
       </c>
       <c r="F177">
@@ -11594,7 +11619,7 @@
       <c r="D178" t="s">
         <v>46</v>
       </c>
-      <c r="E178">
+      <c r="E178" s="2">
         <v>1410</v>
       </c>
       <c r="F178">
@@ -11653,7 +11678,7 @@
       <c r="D179" t="s">
         <v>46</v>
       </c>
-      <c r="E179">
+      <c r="E179" s="2">
         <v>1410</v>
       </c>
       <c r="F179">
@@ -11715,7 +11740,7 @@
       <c r="D180" t="s">
         <v>46</v>
       </c>
-      <c r="E180">
+      <c r="E180" s="2">
         <v>1880</v>
       </c>
       <c r="F180">
@@ -11774,7 +11799,7 @@
       <c r="D181" t="s">
         <v>46</v>
       </c>
-      <c r="E181">
+      <c r="E181" s="2">
         <v>1739</v>
       </c>
       <c r="F181">
@@ -11836,7 +11861,7 @@
       <c r="D182" t="s">
         <v>46</v>
       </c>
-      <c r="E182">
+      <c r="E182" s="2">
         <v>1370</v>
       </c>
       <c r="F182">
@@ -11895,7 +11920,7 @@
       <c r="D183" t="s">
         <v>46</v>
       </c>
-      <c r="E183">
+      <c r="E183" s="2">
         <v>1275</v>
       </c>
       <c r="F183">
@@ -11957,7 +11982,7 @@
       <c r="D184" t="s">
         <v>46</v>
       </c>
-      <c r="E184">
+      <c r="E184" s="2">
         <v>1745</v>
       </c>
       <c r="F184">
@@ -12016,7 +12041,7 @@
       <c r="D185" t="s">
         <v>46</v>
       </c>
-      <c r="E185">
+      <c r="E185" s="2">
         <v>1320.5</v>
       </c>
       <c r="F185">
@@ -12075,7 +12100,7 @@
       <c r="D186" t="s">
         <v>46</v>
       </c>
-      <c r="E186">
+      <c r="E186" s="2">
         <v>1900</v>
       </c>
       <c r="F186">
@@ -12134,7 +12159,7 @@
       <c r="D187" t="s">
         <v>46</v>
       </c>
-      <c r="E187">
+      <c r="E187" s="2">
         <v>1621.5</v>
       </c>
       <c r="F187">
@@ -12193,7 +12218,7 @@
       <c r="D188" t="s">
         <v>46</v>
       </c>
-      <c r="E188">
+      <c r="E188" s="2">
         <v>1292.5</v>
       </c>
       <c r="F188">
@@ -12255,7 +12280,7 @@
       <c r="D189" t="s">
         <v>46</v>
       </c>
-      <c r="E189">
+      <c r="E189" s="2">
         <v>1739</v>
       </c>
       <c r="F189">
@@ -12314,7 +12339,7 @@
       <c r="D190" t="s">
         <v>46</v>
       </c>
-      <c r="E190">
+      <c r="E190" s="2">
         <v>1410</v>
       </c>
       <c r="F190">
@@ -12373,7 +12398,7 @@
       <c r="D191" t="s">
         <v>46</v>
       </c>
-      <c r="E191">
+      <c r="E191" s="2">
         <v>1645</v>
       </c>
       <c r="F191">
@@ -12435,7 +12460,7 @@
       <c r="D192" t="s">
         <v>46</v>
       </c>
-      <c r="E192">
+      <c r="E192" s="2">
         <v>1410</v>
       </c>
       <c r="F192">
@@ -12497,7 +12522,7 @@
       <c r="D193" t="s">
         <v>46</v>
       </c>
-      <c r="E193">
+      <c r="E193" s="2">
         <v>2162</v>
       </c>
       <c r="F193">
@@ -12559,7 +12584,7 @@
       <c r="D194" t="s">
         <v>46</v>
       </c>
-      <c r="E194">
+      <c r="E194" s="2">
         <v>987</v>
       </c>
       <c r="F194">
@@ -12618,7 +12643,7 @@
       <c r="D195" t="s">
         <v>46</v>
       </c>
-      <c r="E195">
+      <c r="E195" s="2">
         <v>1175</v>
       </c>
       <c r="F195">
@@ -12680,7 +12705,7 @@
       <c r="D196" t="s">
         <v>46</v>
       </c>
-      <c r="E196">
+      <c r="E196" s="2">
         <v>1762.5</v>
       </c>
       <c r="F196">
@@ -12739,7 +12764,7 @@
       <c r="D197" t="s">
         <v>46</v>
       </c>
-      <c r="E197">
+      <c r="E197" s="2">
         <v>1645</v>
       </c>
       <c r="F197">
@@ -12798,7 +12823,7 @@
       <c r="D198" t="s">
         <v>46</v>
       </c>
-      <c r="E198">
+      <c r="E198" s="2">
         <v>1527.5</v>
       </c>
       <c r="F198">
@@ -12857,7 +12882,7 @@
       <c r="D199" t="s">
         <v>46</v>
       </c>
-      <c r="E199">
+      <c r="E199" s="2">
         <v>1645</v>
       </c>
       <c r="F199">
@@ -12916,7 +12941,7 @@
       <c r="D200" t="s">
         <v>46</v>
       </c>
-      <c r="E200">
+      <c r="E200" s="2">
         <v>1645</v>
       </c>
       <c r="F200">
@@ -12975,7 +13000,7 @@
       <c r="D201" t="s">
         <v>46</v>
       </c>
-      <c r="E201">
+      <c r="E201" s="2">
         <v>1645</v>
       </c>
       <c r="F201">
@@ -13034,7 +13059,7 @@
       <c r="D202" t="s">
         <v>46</v>
       </c>
-      <c r="E202">
+      <c r="E202" s="2">
         <v>1645</v>
       </c>
       <c r="F202">
@@ -13093,7 +13118,7 @@
       <c r="D203" t="s">
         <v>46</v>
       </c>
-      <c r="E203">
+      <c r="E203" s="2">
         <v>940</v>
       </c>
       <c r="F203">
@@ -13155,7 +13180,7 @@
       <c r="D204" t="s">
         <v>46</v>
       </c>
-      <c r="E204">
+      <c r="E204" s="2">
         <v>1645</v>
       </c>
       <c r="F204">
@@ -13217,7 +13242,7 @@
       <c r="D205" t="s">
         <v>46</v>
       </c>
-      <c r="E205">
+      <c r="E205" s="2">
         <v>1410</v>
       </c>
       <c r="F205">
@@ -13276,7 +13301,7 @@
       <c r="D206" t="s">
         <v>46</v>
       </c>
-      <c r="E206">
+      <c r="E206" s="2">
         <v>1880</v>
       </c>
       <c r="F206">
@@ -13338,7 +13363,7 @@
       <c r="D207" t="s">
         <v>46</v>
       </c>
-      <c r="E207">
+      <c r="E207" s="2">
         <v>1880</v>
       </c>
       <c r="F207">
@@ -13400,7 +13425,7 @@
       <c r="D208" t="s">
         <v>46</v>
       </c>
-      <c r="E208">
+      <c r="E208" s="2">
         <v>1880</v>
       </c>
       <c r="F208">
@@ -13462,7 +13487,7 @@
       <c r="D209" t="s">
         <v>46</v>
       </c>
-      <c r="E209">
+      <c r="E209" s="2">
         <v>1880</v>
       </c>
       <c r="F209">
@@ -13521,7 +13546,7 @@
       <c r="D210" t="s">
         <v>46</v>
       </c>
-      <c r="E210">
+      <c r="E210" s="2">
         <v>1410</v>
       </c>
       <c r="F210">
@@ -13580,7 +13605,7 @@
       <c r="D211" t="s">
         <v>46</v>
       </c>
-      <c r="E211">
+      <c r="E211" s="2">
         <v>1175</v>
       </c>
       <c r="F211">
@@ -13642,7 +13667,7 @@
       <c r="D212" t="s">
         <v>46</v>
       </c>
-      <c r="E212">
+      <c r="E212" s="2">
         <v>2044.5</v>
       </c>
       <c r="F212">
@@ -13704,7 +13729,7 @@
       <c r="D213" t="s">
         <v>46</v>
       </c>
-      <c r="E213">
+      <c r="E213" s="2">
         <v>1175</v>
       </c>
       <c r="F213">
@@ -13763,7 +13788,7 @@
       <c r="D214" t="s">
         <v>46</v>
       </c>
-      <c r="E214">
+      <c r="E214" s="2">
         <v>1527.5</v>
       </c>
       <c r="F214">
@@ -13825,7 +13850,7 @@
       <c r="D215" t="s">
         <v>46</v>
       </c>
-      <c r="E215">
+      <c r="E215" s="2">
         <v>500</v>
       </c>
       <c r="F215">
@@ -13887,7 +13912,7 @@
       <c r="D216" t="s">
         <v>46</v>
       </c>
-      <c r="E216">
+      <c r="E216" s="2">
         <v>1175</v>
       </c>
       <c r="F216">
@@ -13946,7 +13971,7 @@
       <c r="D217" t="s">
         <v>46</v>
       </c>
-      <c r="E217">
+      <c r="E217" s="2">
         <v>1104.5</v>
       </c>
       <c r="F217">
@@ -14008,7 +14033,7 @@
       <c r="D218" t="s">
         <v>46</v>
       </c>
-      <c r="E218">
+      <c r="E218" s="2">
         <v>1175</v>
       </c>
       <c r="F218">
@@ -14067,7 +14092,7 @@
       <c r="D219" t="s">
         <v>46</v>
       </c>
-      <c r="E219">
+      <c r="E219" s="2">
         <v>1410</v>
       </c>
       <c r="F219">
@@ -14129,7 +14154,7 @@
       <c r="D220" t="s">
         <v>46</v>
       </c>
-      <c r="E220">
+      <c r="E220" s="2">
         <v>1175</v>
       </c>
       <c r="F220">
@@ -14191,7 +14216,7 @@
       <c r="D221" t="s">
         <v>46</v>
       </c>
-      <c r="E221">
+      <c r="E221" s="2">
         <v>1175</v>
       </c>
       <c r="F221">
@@ -14250,7 +14275,7 @@
       <c r="D222" t="s">
         <v>46</v>
       </c>
-      <c r="E222">
+      <c r="E222" s="2">
         <v>1175</v>
       </c>
       <c r="F222">
@@ -14312,7 +14337,7 @@
       <c r="D223" t="s">
         <v>46</v>
       </c>
-      <c r="E223">
+      <c r="E223" s="2">
         <v>1645</v>
       </c>
       <c r="F223">
@@ -14371,7 +14396,7 @@
       <c r="D224" t="s">
         <v>46</v>
       </c>
-      <c r="E224">
+      <c r="E224" s="2">
         <v>940</v>
       </c>
       <c r="F224">
@@ -14433,7 +14458,7 @@
       <c r="D225" t="s">
         <v>46</v>
       </c>
-      <c r="E225">
+      <c r="E225" s="2">
         <v>1175</v>
       </c>
       <c r="F225">
@@ -14492,7 +14517,7 @@
       <c r="D226" t="s">
         <v>46</v>
       </c>
-      <c r="E226">
+      <c r="E226" s="2">
         <v>1175</v>
       </c>
       <c r="F226">
@@ -14551,7 +14576,7 @@
       <c r="D227" t="s">
         <v>46</v>
       </c>
-      <c r="E227">
+      <c r="E227" s="2">
         <v>1880</v>
       </c>
       <c r="F227">
@@ -14613,7 +14638,7 @@
       <c r="D228" t="s">
         <v>46</v>
       </c>
-      <c r="E228">
+      <c r="E228" s="2">
         <v>1410</v>
       </c>
       <c r="F228">
@@ -14672,7 +14697,7 @@
       <c r="D229" t="s">
         <v>46</v>
       </c>
-      <c r="E229">
+      <c r="E229" s="2">
         <v>940</v>
       </c>
       <c r="F229">
@@ -14734,7 +14759,7 @@
       <c r="D230" t="s">
         <v>46</v>
       </c>
-      <c r="E230">
+      <c r="E230" s="2">
         <v>940</v>
       </c>
       <c r="F230">
@@ -14793,7 +14818,7 @@
       <c r="D231" t="s">
         <v>46</v>
       </c>
-      <c r="E231">
+      <c r="E231" s="2">
         <v>1175</v>
       </c>
       <c r="F231">
@@ -14855,7 +14880,7 @@
       <c r="D232" t="s">
         <v>46</v>
       </c>
-      <c r="E232">
+      <c r="E232" s="2">
         <v>705</v>
       </c>
       <c r="F232">
@@ -14914,7 +14939,7 @@
       <c r="D233" t="s">
         <v>46</v>
       </c>
-      <c r="E233">
+      <c r="E233" s="2">
         <v>1645</v>
       </c>
       <c r="F233">
@@ -14976,7 +15001,7 @@
       <c r="D234" t="s">
         <v>46</v>
       </c>
-      <c r="E234">
+      <c r="E234" s="2">
         <v>1175</v>
       </c>
       <c r="F234">
@@ -15038,7 +15063,7 @@
       <c r="D235" t="s">
         <v>46</v>
       </c>
-      <c r="E235">
+      <c r="E235" s="2">
         <v>1175</v>
       </c>
       <c r="F235">
@@ -15097,7 +15122,7 @@
       <c r="D236" t="s">
         <v>46</v>
       </c>
-      <c r="E236">
+      <c r="E236" s="2">
         <v>1645</v>
       </c>
       <c r="F236">
@@ -15156,7 +15181,7 @@
       <c r="D237" t="s">
         <v>46</v>
       </c>
-      <c r="E237">
+      <c r="E237" s="2">
         <v>1762.5</v>
       </c>
       <c r="F237">
@@ -15215,7 +15240,7 @@
       <c r="D238" t="s">
         <v>46</v>
       </c>
-      <c r="E238">
+      <c r="E238" s="2">
         <v>2115</v>
       </c>
       <c r="F238">
@@ -15277,7 +15302,7 @@
       <c r="D239" t="s">
         <v>46</v>
       </c>
-      <c r="E239">
+      <c r="E239" s="2">
         <v>1410</v>
       </c>
       <c r="F239">
@@ -15336,7 +15361,7 @@
       <c r="D240" t="s">
         <v>46</v>
       </c>
-      <c r="E240">
+      <c r="E240" s="2">
         <v>1880</v>
       </c>
       <c r="F240">
@@ -15398,7 +15423,7 @@
       <c r="D241" t="s">
         <v>46</v>
       </c>
-      <c r="E241">
+      <c r="E241" s="2">
         <v>2820</v>
       </c>
       <c r="F241">
@@ -15457,7 +15482,7 @@
       <c r="D242" t="s">
         <v>46</v>
       </c>
-      <c r="E242">
+      <c r="E242" s="2">
         <v>1645</v>
       </c>
       <c r="F242">
@@ -15516,7 +15541,7 @@
       <c r="D243" t="s">
         <v>46</v>
       </c>
-      <c r="E243">
+      <c r="E243" s="2">
         <v>1903.5</v>
       </c>
       <c r="F243">
@@ -15575,7 +15600,7 @@
       <c r="D244" t="s">
         <v>46</v>
       </c>
-      <c r="E244">
+      <c r="E244" s="2">
         <v>1997.5</v>
       </c>
       <c r="F244">
@@ -15634,7 +15659,7 @@
       <c r="D245" t="s">
         <v>46</v>
       </c>
-      <c r="E245">
+      <c r="E245" s="2">
         <v>1880</v>
       </c>
       <c r="F245">
@@ -15696,7 +15721,7 @@
       <c r="D246" t="s">
         <v>46</v>
       </c>
-      <c r="E246">
+      <c r="E246" s="2">
         <v>1715.5</v>
       </c>
       <c r="F246">

</xml_diff>